<commit_message>
Implementación original y memético (buenos resultados)
</commit_message>
<xml_diff>
--- a/Proyecto_Final/Código/results_ant_lion/results_cec2017_10.xlsx
+++ b/Proyecto_Final/Código/results_ant_lion/results_cec2017_10.xlsx
@@ -579,94 +579,94 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>16571193700</v>
+        <v>6146854600</v>
       </c>
       <c r="D2">
-        <v>79573461330000</v>
+        <v>358642617100</v>
       </c>
       <c r="E2">
-        <v>80511.00499999999</v>
+        <v>42286.361</v>
       </c>
       <c r="F2">
-        <v>2494.89189</v>
+        <v>564.27208</v>
       </c>
       <c r="G2">
-        <v>149.06841</v>
+        <v>98.61119299999999</v>
       </c>
       <c r="H2">
-        <v>99.980987</v>
+        <v>71.746882</v>
       </c>
       <c r="I2">
-        <v>399.2386</v>
+        <v>341.16292</v>
       </c>
       <c r="J2">
-        <v>144.51851</v>
+        <v>109.428626</v>
       </c>
       <c r="K2">
-        <v>3707.9775</v>
+        <v>2788.2442</v>
       </c>
       <c r="L2">
-        <v>2492.267</v>
+        <v>1915.3584</v>
       </c>
       <c r="M2">
-        <v>14679.5688</v>
+        <v>1964.11202</v>
       </c>
       <c r="N2">
-        <v>2405794170</v>
+        <v>395216213</v>
       </c>
       <c r="O2">
-        <v>217149200</v>
+        <v>8084390.3</v>
       </c>
       <c r="P2">
-        <v>5114651.6071</v>
+        <v>25545.8843</v>
       </c>
       <c r="Q2">
-        <v>26336324.388</v>
+        <v>174938.3251</v>
       </c>
       <c r="R2">
-        <v>1062.33061</v>
+        <v>506.8584</v>
       </c>
       <c r="S2">
-        <v>639.92233</v>
+        <v>316.90687</v>
       </c>
       <c r="T2">
-        <v>625437850</v>
+        <v>8393094.190000001</v>
       </c>
       <c r="U2">
-        <v>40718105.96</v>
+        <v>638273.9069999999</v>
       </c>
       <c r="V2">
-        <v>552.09223</v>
+        <v>383.27676</v>
       </c>
       <c r="W2">
-        <v>333.92859</v>
+        <v>284.42671</v>
       </c>
       <c r="X2">
-        <v>1836.715</v>
+        <v>1094.73898</v>
       </c>
       <c r="Y2">
-        <v>540.2689699999999</v>
+        <v>379.12055</v>
       </c>
       <c r="Z2">
-        <v>584.18386</v>
+        <v>401.51096</v>
       </c>
       <c r="AA2">
-        <v>1976.8844</v>
+        <v>771.4745</v>
       </c>
       <c r="AB2">
-        <v>2158.7314</v>
+        <v>1230.92392</v>
       </c>
       <c r="AC2">
-        <v>688.07339</v>
+        <v>414.4614</v>
       </c>
       <c r="AD2">
-        <v>1253.73054</v>
+        <v>651.6048400000001</v>
       </c>
       <c r="AE2">
-        <v>910.44229</v>
+        <v>588.59416</v>
       </c>
       <c r="AF2">
-        <v>136807693</v>
+        <v>5361469.96</v>
       </c>
       <c r="AG2">
         <v>10</v>
@@ -680,94 +680,94 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>16571193700</v>
+        <v>5224661900</v>
       </c>
       <c r="D3">
-        <v>79573461330000</v>
+        <v>106230884926.1</v>
       </c>
       <c r="E3">
-        <v>80511.00499999999</v>
+        <v>31441.356</v>
       </c>
       <c r="F3">
-        <v>2494.89189</v>
+        <v>388.28076</v>
       </c>
       <c r="G3">
-        <v>149.06841</v>
+        <v>91.94196699999999</v>
       </c>
       <c r="H3">
-        <v>99.980987</v>
+        <v>53.857941</v>
       </c>
       <c r="I3">
-        <v>399.2386</v>
+        <v>315.5824</v>
       </c>
       <c r="J3">
-        <v>144.51851</v>
+        <v>102.170887</v>
       </c>
       <c r="K3">
-        <v>3707.9775</v>
+        <v>2244.84641</v>
       </c>
       <c r="L3">
-        <v>2492.267</v>
+        <v>1848.8512</v>
       </c>
       <c r="M3">
-        <v>14679.5688</v>
+        <v>959.5705700000002</v>
       </c>
       <c r="N3">
-        <v>2405794170</v>
+        <v>239486223</v>
       </c>
       <c r="O3">
-        <v>217149200</v>
+        <v>4356647.430000001</v>
       </c>
       <c r="P3">
-        <v>5114651.6071</v>
+        <v>4967.7998</v>
       </c>
       <c r="Q3">
-        <v>26336324.388</v>
+        <v>90123.73510000001</v>
       </c>
       <c r="R3">
-        <v>1062.33061</v>
+        <v>405.2687200000001</v>
       </c>
       <c r="S3">
-        <v>639.92233</v>
+        <v>290.99742</v>
       </c>
       <c r="T3">
-        <v>625437850</v>
+        <v>2735681.06</v>
       </c>
       <c r="U3">
-        <v>40718105.96</v>
+        <v>114376.147</v>
       </c>
       <c r="V3">
-        <v>552.09223</v>
+        <v>359.888</v>
       </c>
       <c r="W3">
-        <v>333.92859</v>
+        <v>280.04993</v>
       </c>
       <c r="X3">
-        <v>1836.715</v>
+        <v>866.15007</v>
       </c>
       <c r="Y3">
-        <v>540.2689699999999</v>
+        <v>376.38416</v>
       </c>
       <c r="Z3">
-        <v>584.18386</v>
+        <v>396.12491</v>
       </c>
       <c r="AA3">
-        <v>1976.8844</v>
+        <v>631.40703</v>
       </c>
       <c r="AB3">
-        <v>2158.7314</v>
+        <v>1043.58825</v>
       </c>
       <c r="AC3">
-        <v>688.07339</v>
+        <v>409.85814</v>
       </c>
       <c r="AD3">
-        <v>1253.73054</v>
+        <v>590.99479</v>
       </c>
       <c r="AE3">
-        <v>910.44229</v>
+        <v>484.1404899999999</v>
       </c>
       <c r="AF3">
-        <v>136807693</v>
+        <v>2134710.14</v>
       </c>
       <c r="AG3">
         <v>10</v>
@@ -781,94 +781,94 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>16571193700</v>
+        <v>4505800100</v>
       </c>
       <c r="D4">
-        <v>79573461330000</v>
+        <v>66025926726.1</v>
       </c>
       <c r="E4">
-        <v>80511.00499999999</v>
+        <v>30264.567</v>
       </c>
       <c r="F4">
-        <v>2494.89189</v>
+        <v>355.57983</v>
       </c>
       <c r="G4">
-        <v>149.06841</v>
+        <v>87.94027800000001</v>
       </c>
       <c r="H4">
-        <v>99.980987</v>
+        <v>48.175964</v>
       </c>
       <c r="I4">
-        <v>399.2386</v>
+        <v>287.1773400000001</v>
       </c>
       <c r="J4">
-        <v>144.51851</v>
+        <v>96.07555599999999</v>
       </c>
       <c r="K4">
-        <v>3707.9775</v>
+        <v>2013.61779</v>
       </c>
       <c r="L4">
-        <v>2492.267</v>
+        <v>1718.8183</v>
       </c>
       <c r="M4">
-        <v>14679.5688</v>
+        <v>872.9395000000001</v>
       </c>
       <c r="N4">
-        <v>2405794170</v>
+        <v>181013275</v>
       </c>
       <c r="O4">
-        <v>217149200</v>
+        <v>837174.335</v>
       </c>
       <c r="P4">
-        <v>5114651.6071</v>
+        <v>4967.7998</v>
       </c>
       <c r="Q4">
-        <v>26336324.388</v>
+        <v>85367.28580000001</v>
       </c>
       <c r="R4">
-        <v>1062.33061</v>
+        <v>379.33846</v>
       </c>
       <c r="S4">
-        <v>639.92233</v>
+        <v>278.05295</v>
       </c>
       <c r="T4">
-        <v>625437850</v>
+        <v>2017110.96</v>
       </c>
       <c r="U4">
-        <v>40718105.96</v>
+        <v>76197.322</v>
       </c>
       <c r="V4">
-        <v>552.09223</v>
+        <v>311.95251</v>
       </c>
       <c r="W4">
-        <v>333.92859</v>
+        <v>273.11464</v>
       </c>
       <c r="X4">
-        <v>1836.715</v>
+        <v>770.9872099999999</v>
       </c>
       <c r="Y4">
-        <v>540.2689699999999</v>
+        <v>373.50426</v>
       </c>
       <c r="Z4">
-        <v>584.18386</v>
+        <v>393.93556</v>
       </c>
       <c r="AA4">
-        <v>1976.8844</v>
+        <v>615.6946799999999</v>
       </c>
       <c r="AB4">
-        <v>2158.7314</v>
+        <v>961.1867199999999</v>
       </c>
       <c r="AC4">
-        <v>688.07339</v>
+        <v>407.9494</v>
       </c>
       <c r="AD4">
-        <v>1253.73054</v>
+        <v>565.6419699999999</v>
       </c>
       <c r="AE4">
-        <v>910.44229</v>
+        <v>467.9005099999999</v>
       </c>
       <c r="AF4">
-        <v>136807693</v>
+        <v>1860319.44</v>
       </c>
       <c r="AG4">
         <v>10</v>
@@ -882,94 +882,94 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>16571193700</v>
+        <v>3743717000</v>
       </c>
       <c r="D5">
-        <v>79573461330000</v>
+        <v>55422748726.1</v>
       </c>
       <c r="E5">
-        <v>80511.00499999999</v>
+        <v>28015.11700000001</v>
       </c>
       <c r="F5">
-        <v>2494.89189</v>
+        <v>278.61871</v>
       </c>
       <c r="G5">
-        <v>149.06841</v>
+        <v>85.301064</v>
       </c>
       <c r="H5">
-        <v>99.980987</v>
+        <v>44.16897099999999</v>
       </c>
       <c r="I5">
-        <v>399.2386</v>
+        <v>281.6633</v>
       </c>
       <c r="J5">
-        <v>144.51851</v>
+        <v>90.003693</v>
       </c>
       <c r="K5">
-        <v>3707.9775</v>
+        <v>1653.11109</v>
       </c>
       <c r="L5">
-        <v>2492.267</v>
+        <v>1637.6215</v>
       </c>
       <c r="M5">
-        <v>14679.5688</v>
+        <v>673.91961</v>
       </c>
       <c r="N5">
-        <v>2405794170</v>
+        <v>120859300</v>
       </c>
       <c r="O5">
-        <v>217149200</v>
+        <v>384718.564</v>
       </c>
       <c r="P5">
-        <v>5114651.6071</v>
+        <v>2936.57091</v>
       </c>
       <c r="Q5">
-        <v>26336324.388</v>
+        <v>38260.4569</v>
       </c>
       <c r="R5">
-        <v>1062.33061</v>
+        <v>305.51715</v>
       </c>
       <c r="S5">
-        <v>639.92233</v>
+        <v>227.4650599999999</v>
       </c>
       <c r="T5">
-        <v>625437850</v>
+        <v>872809.0299999999</v>
       </c>
       <c r="U5">
-        <v>40718105.96</v>
+        <v>46445.461</v>
       </c>
       <c r="V5">
-        <v>552.09223</v>
+        <v>276.50904</v>
       </c>
       <c r="W5">
-        <v>333.92859</v>
+        <v>254.62399</v>
       </c>
       <c r="X5">
-        <v>1836.715</v>
+        <v>635.20185</v>
       </c>
       <c r="Y5">
-        <v>540.2689699999999</v>
+        <v>366.8684999999999</v>
       </c>
       <c r="Z5">
-        <v>584.18386</v>
+        <v>387.2735</v>
       </c>
       <c r="AA5">
-        <v>1976.8844</v>
+        <v>592.30643</v>
       </c>
       <c r="AB5">
-        <v>2158.7314</v>
+        <v>821.7347599999999</v>
       </c>
       <c r="AC5">
-        <v>688.07339</v>
+        <v>405.5393400000001</v>
       </c>
       <c r="AD5">
-        <v>1253.73054</v>
+        <v>558.43728</v>
       </c>
       <c r="AE5">
-        <v>910.44229</v>
+        <v>408.20374</v>
       </c>
       <c r="AF5">
-        <v>136807693</v>
+        <v>1433680.97</v>
       </c>
       <c r="AG5">
         <v>10</v>
@@ -983,94 +983,94 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>16571193700</v>
+        <v>2769738400</v>
       </c>
       <c r="D6">
-        <v>79573461330000</v>
+        <v>10951393046.1</v>
       </c>
       <c r="E6">
-        <v>80511.00499999999</v>
+        <v>23991.906</v>
       </c>
       <c r="F6">
-        <v>2494.89189</v>
+        <v>201.448888</v>
       </c>
       <c r="G6">
-        <v>149.06841</v>
+        <v>71.42121499999999</v>
       </c>
       <c r="H6">
-        <v>99.980987</v>
+        <v>36.63771</v>
       </c>
       <c r="I6">
-        <v>399.2386</v>
+        <v>211.13934</v>
       </c>
       <c r="J6">
-        <v>144.51851</v>
+        <v>82.94570999999999</v>
       </c>
       <c r="K6">
-        <v>3707.9775</v>
+        <v>1213.77239</v>
       </c>
       <c r="L6">
-        <v>2492.267</v>
+        <v>1525.4197</v>
       </c>
       <c r="M6">
-        <v>14679.5688</v>
+        <v>407.56433</v>
       </c>
       <c r="N6">
-        <v>2405794170</v>
+        <v>72660977</v>
       </c>
       <c r="O6">
-        <v>217149200</v>
+        <v>168822.495</v>
       </c>
       <c r="P6">
-        <v>5114651.6071</v>
+        <v>1783.69</v>
       </c>
       <c r="Q6">
-        <v>26336324.388</v>
+        <v>36424.0417</v>
       </c>
       <c r="R6">
-        <v>1062.33061</v>
+        <v>224.8744000000001</v>
       </c>
       <c r="S6">
-        <v>639.92233</v>
+        <v>146.445919</v>
       </c>
       <c r="T6">
-        <v>625437850</v>
+        <v>659525.3860000002</v>
       </c>
       <c r="U6">
-        <v>40718105.96</v>
+        <v>34916.72100000001</v>
       </c>
       <c r="V6">
-        <v>552.09223</v>
+        <v>211.40527</v>
       </c>
       <c r="W6">
-        <v>333.92859</v>
+        <v>228.71183</v>
       </c>
       <c r="X6">
-        <v>1836.715</v>
+        <v>389.61679</v>
       </c>
       <c r="Y6">
-        <v>540.2689699999999</v>
+        <v>360.96239</v>
       </c>
       <c r="Z6">
-        <v>584.18386</v>
+        <v>379.45274</v>
       </c>
       <c r="AA6">
-        <v>1976.8844</v>
+        <v>576.4212</v>
       </c>
       <c r="AB6">
-        <v>2158.7314</v>
+        <v>734.0136399999999</v>
       </c>
       <c r="AC6">
-        <v>688.07339</v>
+        <v>402.56604</v>
       </c>
       <c r="AD6">
-        <v>1253.73054</v>
+        <v>552.8605</v>
       </c>
       <c r="AE6">
-        <v>910.44229</v>
+        <v>373.95503</v>
       </c>
       <c r="AF6">
-        <v>136807693</v>
+        <v>1165339.79</v>
       </c>
       <c r="AG6">
         <v>10</v>
@@ -1084,94 +1084,94 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>16571193700</v>
+        <v>2186104500</v>
       </c>
       <c r="D7">
-        <v>79573461330000</v>
+        <v>1799920588.1</v>
       </c>
       <c r="E7">
-        <v>80511.00499999999</v>
+        <v>13387.5411</v>
       </c>
       <c r="F7">
-        <v>2494.89189</v>
+        <v>117.553439</v>
       </c>
       <c r="G7">
-        <v>149.06841</v>
+        <v>63.773888</v>
       </c>
       <c r="H7">
-        <v>99.980987</v>
+        <v>31.806436</v>
       </c>
       <c r="I7">
-        <v>399.2386</v>
+        <v>163.39122</v>
       </c>
       <c r="J7">
-        <v>144.51851</v>
+        <v>75.37098300000001</v>
       </c>
       <c r="K7">
-        <v>3707.9775</v>
+        <v>962.97657</v>
       </c>
       <c r="L7">
-        <v>2492.267</v>
+        <v>1282.02222</v>
       </c>
       <c r="M7">
-        <v>14679.5688</v>
+        <v>301.592554</v>
       </c>
       <c r="N7">
-        <v>2405794170</v>
+        <v>30470234.4</v>
       </c>
       <c r="O7">
-        <v>217149200</v>
+        <v>68317.376</v>
       </c>
       <c r="P7">
-        <v>5114651.6071</v>
+        <v>1046.67595</v>
       </c>
       <c r="Q7">
-        <v>26336324.388</v>
+        <v>7900.418790000001</v>
       </c>
       <c r="R7">
-        <v>1062.33061</v>
+        <v>174.383684</v>
       </c>
       <c r="S7">
-        <v>639.92233</v>
+        <v>107.721576</v>
       </c>
       <c r="T7">
-        <v>625437850</v>
+        <v>526872.9180000001</v>
       </c>
       <c r="U7">
-        <v>40718105.96</v>
+        <v>29810.557</v>
       </c>
       <c r="V7">
-        <v>552.09223</v>
+        <v>169.20877</v>
       </c>
       <c r="W7">
-        <v>333.92859</v>
+        <v>187.88517</v>
       </c>
       <c r="X7">
-        <v>1836.715</v>
+        <v>309.91858</v>
       </c>
       <c r="Y7">
-        <v>540.2689699999999</v>
+        <v>355.4949799999999</v>
       </c>
       <c r="Z7">
-        <v>584.18386</v>
+        <v>376.42845</v>
       </c>
       <c r="AA7">
-        <v>1976.8844</v>
+        <v>546.42227</v>
       </c>
       <c r="AB7">
-        <v>2158.7314</v>
+        <v>669.17127</v>
       </c>
       <c r="AC7">
-        <v>688.07339</v>
+        <v>400.91094</v>
       </c>
       <c r="AD7">
-        <v>1253.73054</v>
+        <v>525.0671099999998</v>
       </c>
       <c r="AE7">
-        <v>910.44229</v>
+        <v>349.02966</v>
       </c>
       <c r="AF7">
-        <v>136807693</v>
+        <v>809344.26</v>
       </c>
       <c r="AG7">
         <v>10</v>
@@ -1185,94 +1185,94 @@
         <v>30</v>
       </c>
       <c r="C8">
-        <v>16571193700</v>
+        <v>1657251500</v>
       </c>
       <c r="D8">
-        <v>79573461330000</v>
+        <v>1624712613.5</v>
       </c>
       <c r="E8">
-        <v>80511.00499999999</v>
+        <v>9938.5874</v>
       </c>
       <c r="F8">
-        <v>2494.89189</v>
+        <v>72.087386</v>
       </c>
       <c r="G8">
-        <v>149.06841</v>
+        <v>58.532382</v>
       </c>
       <c r="H8">
-        <v>99.980987</v>
+        <v>26.165477</v>
       </c>
       <c r="I8">
-        <v>399.2386</v>
+        <v>144.10308</v>
       </c>
       <c r="J8">
-        <v>144.51851</v>
+        <v>69.461349</v>
       </c>
       <c r="K8">
-        <v>3707.9775</v>
+        <v>782.95286</v>
       </c>
       <c r="L8">
-        <v>2492.267</v>
+        <v>1232.71617</v>
       </c>
       <c r="M8">
-        <v>14679.5688</v>
+        <v>226.222284</v>
       </c>
       <c r="N8">
-        <v>2405794170</v>
+        <v>14337124.8</v>
       </c>
       <c r="O8">
-        <v>217149200</v>
+        <v>27199.4641</v>
       </c>
       <c r="P8">
-        <v>5114651.6071</v>
+        <v>627.88126</v>
       </c>
       <c r="Q8">
-        <v>26336324.388</v>
+        <v>4975.19069</v>
       </c>
       <c r="R8">
-        <v>1062.33061</v>
+        <v>134.835222</v>
       </c>
       <c r="S8">
-        <v>639.92233</v>
+        <v>97.790515</v>
       </c>
       <c r="T8">
-        <v>625437850</v>
+        <v>507458.6850000002</v>
       </c>
       <c r="U8">
-        <v>40718105.96</v>
+        <v>23980.388</v>
       </c>
       <c r="V8">
-        <v>552.09223</v>
+        <v>154.748031</v>
       </c>
       <c r="W8">
-        <v>333.92859</v>
+        <v>158.43592</v>
       </c>
       <c r="X8">
-        <v>1836.715</v>
+        <v>276.78042</v>
       </c>
       <c r="Y8">
-        <v>540.2689699999999</v>
+        <v>351.05725</v>
       </c>
       <c r="Z8">
-        <v>584.18386</v>
+        <v>373.55274</v>
       </c>
       <c r="AA8">
-        <v>1976.8844</v>
+        <v>525.675</v>
       </c>
       <c r="AB8">
-        <v>2158.7314</v>
+        <v>640.4809600000001</v>
       </c>
       <c r="AC8">
-        <v>688.07339</v>
+        <v>400.57048</v>
       </c>
       <c r="AD8">
-        <v>1253.73054</v>
+        <v>518.2833800000001</v>
       </c>
       <c r="AE8">
-        <v>910.44229</v>
+        <v>335.02503</v>
       </c>
       <c r="AF8">
-        <v>136807693</v>
+        <v>753157.72</v>
       </c>
       <c r="AG8">
         <v>10</v>
@@ -1286,94 +1286,94 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>16571193700</v>
+        <v>1453817500</v>
       </c>
       <c r="D9">
-        <v>79573461330000</v>
+        <v>719947673.5</v>
       </c>
       <c r="E9">
-        <v>80511.00499999999</v>
+        <v>6146.1393</v>
       </c>
       <c r="F9">
-        <v>2494.89189</v>
+        <v>62.07145999999999</v>
       </c>
       <c r="G9">
-        <v>149.06841</v>
+        <v>52.49007</v>
       </c>
       <c r="H9">
-        <v>99.980987</v>
+        <v>24.355885</v>
       </c>
       <c r="I9">
-        <v>399.2386</v>
+        <v>127.24488</v>
       </c>
       <c r="J9">
-        <v>144.51851</v>
+        <v>64.098473</v>
       </c>
       <c r="K9">
-        <v>3707.9775</v>
+        <v>488.37652</v>
       </c>
       <c r="L9">
-        <v>2492.267</v>
+        <v>1134.84536</v>
       </c>
       <c r="M9">
-        <v>14679.5688</v>
+        <v>216.371224</v>
       </c>
       <c r="N9">
-        <v>2405794170</v>
+        <v>13802110.58</v>
       </c>
       <c r="O9">
-        <v>217149200</v>
+        <v>25087.6031</v>
       </c>
       <c r="P9">
-        <v>5114651.6071</v>
+        <v>562.74573</v>
       </c>
       <c r="Q9">
-        <v>26336324.388</v>
+        <v>4414.22429</v>
       </c>
       <c r="R9">
-        <v>1062.33061</v>
+        <v>117.389926</v>
       </c>
       <c r="S9">
-        <v>639.92233</v>
+        <v>93.22083600000001</v>
       </c>
       <c r="T9">
-        <v>625437850</v>
+        <v>492537.849</v>
       </c>
       <c r="U9">
-        <v>40718105.96</v>
+        <v>21737.5965</v>
       </c>
       <c r="V9">
-        <v>552.09223</v>
+        <v>135.889634</v>
       </c>
       <c r="W9">
-        <v>333.92859</v>
+        <v>154.62502</v>
       </c>
       <c r="X9">
-        <v>1836.715</v>
+        <v>274.0602</v>
       </c>
       <c r="Y9">
-        <v>540.2689699999999</v>
+        <v>349.0534</v>
       </c>
       <c r="Z9">
-        <v>584.18386</v>
+        <v>369.5795200000001</v>
       </c>
       <c r="AA9">
-        <v>1976.8844</v>
+        <v>516.38434</v>
       </c>
       <c r="AB9">
-        <v>2158.7314</v>
+        <v>510.06645</v>
       </c>
       <c r="AC9">
-        <v>688.07339</v>
+        <v>399.67445</v>
       </c>
       <c r="AD9">
-        <v>1253.73054</v>
+        <v>515.2186399999999</v>
       </c>
       <c r="AE9">
-        <v>910.44229</v>
+        <v>320.54236</v>
       </c>
       <c r="AF9">
-        <v>136807693</v>
+        <v>715698.41</v>
       </c>
       <c r="AG9">
         <v>10</v>
@@ -1387,94 +1387,94 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>16571193700</v>
+        <v>1061461070</v>
       </c>
       <c r="D10">
-        <v>79573461330000</v>
+        <v>213709884</v>
       </c>
       <c r="E10">
-        <v>80511.00499999999</v>
+        <v>4529.6335</v>
       </c>
       <c r="F10">
-        <v>2494.89189</v>
+        <v>53.83824599999999</v>
       </c>
       <c r="G10">
-        <v>149.06841</v>
+        <v>48.585435</v>
       </c>
       <c r="H10">
-        <v>99.980987</v>
+        <v>21.48154</v>
       </c>
       <c r="I10">
-        <v>399.2386</v>
+        <v>109.152297</v>
       </c>
       <c r="J10">
-        <v>144.51851</v>
+        <v>56.73565400000001</v>
       </c>
       <c r="K10">
-        <v>3707.9775</v>
+        <v>408.05364</v>
       </c>
       <c r="L10">
-        <v>2492.267</v>
+        <v>1087.45259</v>
       </c>
       <c r="M10">
-        <v>14679.5688</v>
+        <v>145.567771</v>
       </c>
       <c r="N10">
-        <v>2405794170</v>
+        <v>5733951.88</v>
       </c>
       <c r="O10">
-        <v>217149200</v>
+        <v>16713.7917</v>
       </c>
       <c r="P10">
-        <v>5114651.6071</v>
+        <v>382.8492600000001</v>
       </c>
       <c r="Q10">
-        <v>26336324.388</v>
+        <v>3476.56379</v>
       </c>
       <c r="R10">
-        <v>1062.33061</v>
+        <v>107.172251</v>
       </c>
       <c r="S10">
-        <v>639.92233</v>
+        <v>88.59269099999999</v>
       </c>
       <c r="T10">
-        <v>625437850</v>
+        <v>54605.13300000001</v>
       </c>
       <c r="U10">
-        <v>40718105.96</v>
+        <v>17190.1768</v>
       </c>
       <c r="V10">
-        <v>552.09223</v>
+        <v>127.691871</v>
       </c>
       <c r="W10">
-        <v>333.92859</v>
+        <v>154.06411</v>
       </c>
       <c r="X10">
-        <v>1836.715</v>
+        <v>223.09403</v>
       </c>
       <c r="Y10">
-        <v>540.2689699999999</v>
+        <v>347.5628</v>
       </c>
       <c r="Z10">
-        <v>584.18386</v>
+        <v>367.01466</v>
       </c>
       <c r="AA10">
-        <v>1976.8844</v>
+        <v>505.29968</v>
       </c>
       <c r="AB10">
-        <v>2158.7314</v>
+        <v>486.44629</v>
       </c>
       <c r="AC10">
-        <v>688.07339</v>
+        <v>398.70494</v>
       </c>
       <c r="AD10">
-        <v>1253.73054</v>
+        <v>512.75362</v>
       </c>
       <c r="AE10">
-        <v>910.44229</v>
+        <v>304.145</v>
       </c>
       <c r="AF10">
-        <v>136807693</v>
+        <v>579008.4100000001</v>
       </c>
       <c r="AG10">
         <v>10</v>
@@ -1488,94 +1488,94 @@
         <v>60</v>
       </c>
       <c r="C11">
-        <v>16571193700</v>
+        <v>789454900</v>
       </c>
       <c r="D11">
-        <v>79573461330000</v>
+        <v>179197076.4</v>
       </c>
       <c r="E11">
-        <v>80511.00499999999</v>
+        <v>3642.8375</v>
       </c>
       <c r="F11">
-        <v>2494.89189</v>
+        <v>44.86771700000001</v>
       </c>
       <c r="G11">
-        <v>149.06841</v>
+        <v>45.190137</v>
       </c>
       <c r="H11">
-        <v>99.980987</v>
+        <v>18.62865900000001</v>
       </c>
       <c r="I11">
-        <v>399.2386</v>
+        <v>103.386337</v>
       </c>
       <c r="J11">
-        <v>144.51851</v>
+        <v>53.27656399999999</v>
       </c>
       <c r="K11">
-        <v>3707.9775</v>
+        <v>273.65028</v>
       </c>
       <c r="L11">
-        <v>2492.267</v>
+        <v>1076.94119</v>
       </c>
       <c r="M11">
-        <v>14679.5688</v>
+        <v>110.760243</v>
       </c>
       <c r="N11">
-        <v>2405794170</v>
+        <v>4464945.67</v>
       </c>
       <c r="O11">
-        <v>217149200</v>
+        <v>15094.094</v>
       </c>
       <c r="P11">
-        <v>5114651.6071</v>
+        <v>289.53767</v>
       </c>
       <c r="Q11">
-        <v>26336324.388</v>
+        <v>2227.89251</v>
       </c>
       <c r="R11">
-        <v>1062.33061</v>
+        <v>93.59538700000002</v>
       </c>
       <c r="S11">
-        <v>639.92233</v>
+        <v>84.03599799999999</v>
       </c>
       <c r="T11">
-        <v>625437850</v>
+        <v>36112.434</v>
       </c>
       <c r="U11">
-        <v>40718105.96</v>
+        <v>10835.884</v>
       </c>
       <c r="V11">
-        <v>552.09223</v>
+        <v>120.041439</v>
       </c>
       <c r="W11">
-        <v>333.92859</v>
+        <v>150.58955</v>
       </c>
       <c r="X11">
-        <v>1836.715</v>
+        <v>177.34071</v>
       </c>
       <c r="Y11">
-        <v>540.2689699999999</v>
+        <v>343.5416999999999</v>
       </c>
       <c r="Z11">
-        <v>584.18386</v>
+        <v>363.92221</v>
       </c>
       <c r="AA11">
-        <v>1976.8844</v>
+        <v>500.10223</v>
       </c>
       <c r="AB11">
-        <v>2158.7314</v>
+        <v>478.55189</v>
       </c>
       <c r="AC11">
-        <v>688.07339</v>
+        <v>397.88178</v>
       </c>
       <c r="AD11">
-        <v>1253.73054</v>
+        <v>507.19151</v>
       </c>
       <c r="AE11">
-        <v>910.44229</v>
+        <v>300.67249</v>
       </c>
       <c r="AF11">
-        <v>136807693</v>
+        <v>506261.4349999999</v>
       </c>
       <c r="AG11">
         <v>10</v>
@@ -1589,94 +1589,94 @@
         <v>70</v>
       </c>
       <c r="C12">
-        <v>16571193700</v>
+        <v>756773960</v>
       </c>
       <c r="D12">
-        <v>79573461330000</v>
+        <v>90559836.09999999</v>
       </c>
       <c r="E12">
-        <v>80511.00499999999</v>
+        <v>2352.9426</v>
       </c>
       <c r="F12">
-        <v>2494.89189</v>
+        <v>29.569004</v>
       </c>
       <c r="G12">
-        <v>149.06841</v>
+        <v>40.14549100000001</v>
       </c>
       <c r="H12">
-        <v>99.980987</v>
+        <v>15.464793</v>
       </c>
       <c r="I12">
-        <v>399.2386</v>
+        <v>88.55706600000001</v>
       </c>
       <c r="J12">
-        <v>144.51851</v>
+        <v>45.359225</v>
       </c>
       <c r="K12">
-        <v>3707.9775</v>
+        <v>186.65142</v>
       </c>
       <c r="L12">
-        <v>2492.267</v>
+        <v>1020.6835</v>
       </c>
       <c r="M12">
-        <v>14679.5688</v>
+        <v>103.151784</v>
       </c>
       <c r="N12">
-        <v>2405794170</v>
+        <v>3097521.92</v>
       </c>
       <c r="O12">
-        <v>217149200</v>
+        <v>13891.2119</v>
       </c>
       <c r="P12">
-        <v>5114651.6071</v>
+        <v>269.60042</v>
       </c>
       <c r="Q12">
-        <v>26336324.388</v>
+        <v>1718.0427</v>
       </c>
       <c r="R12">
-        <v>1062.33061</v>
+        <v>86.92363</v>
       </c>
       <c r="S12">
-        <v>639.92233</v>
+        <v>79.25284500000001</v>
       </c>
       <c r="T12">
-        <v>625437850</v>
+        <v>32733.461</v>
       </c>
       <c r="U12">
-        <v>40718105.96</v>
+        <v>5849.594999999999</v>
       </c>
       <c r="V12">
-        <v>552.09223</v>
+        <v>119.190391</v>
       </c>
       <c r="W12">
-        <v>333.92859</v>
+        <v>149.2006</v>
       </c>
       <c r="X12">
-        <v>1836.715</v>
+        <v>160.48991</v>
       </c>
       <c r="Y12">
-        <v>540.2689699999999</v>
+        <v>340.32479</v>
       </c>
       <c r="Z12">
-        <v>584.18386</v>
+        <v>359.1847300000001</v>
       </c>
       <c r="AA12">
-        <v>1976.8844</v>
+        <v>475.80407</v>
       </c>
       <c r="AB12">
-        <v>2158.7314</v>
+        <v>455.86726</v>
       </c>
       <c r="AC12">
-        <v>688.07339</v>
+        <v>396.44216</v>
       </c>
       <c r="AD12">
-        <v>1253.73054</v>
+        <v>502.43443</v>
       </c>
       <c r="AE12">
-        <v>910.44229</v>
+        <v>289.68174</v>
       </c>
       <c r="AF12">
-        <v>136807693</v>
+        <v>451436.058</v>
       </c>
       <c r="AG12">
         <v>10</v>
@@ -1690,94 +1690,94 @@
         <v>80</v>
       </c>
       <c r="C13">
-        <v>16571193700</v>
+        <v>444310500</v>
       </c>
       <c r="D13">
-        <v>79573461330000</v>
+        <v>62823571.5</v>
       </c>
       <c r="E13">
-        <v>80511.00499999999</v>
+        <v>1438.80593</v>
       </c>
       <c r="F13">
-        <v>2494.89189</v>
+        <v>23.195443</v>
       </c>
       <c r="G13">
-        <v>149.06841</v>
+        <v>36.1052</v>
       </c>
       <c r="H13">
-        <v>99.980987</v>
+        <v>11.0551667</v>
       </c>
       <c r="I13">
-        <v>399.2386</v>
+        <v>79.048309</v>
       </c>
       <c r="J13">
-        <v>144.51851</v>
+        <v>39.158927</v>
       </c>
       <c r="K13">
-        <v>3707.9775</v>
+        <v>115.086767</v>
       </c>
       <c r="L13">
-        <v>2492.267</v>
+        <v>952.82834</v>
       </c>
       <c r="M13">
-        <v>14679.5688</v>
+        <v>102.152263</v>
       </c>
       <c r="N13">
-        <v>2405794170</v>
+        <v>2563550.47</v>
       </c>
       <c r="O13">
-        <v>217149200</v>
+        <v>12742.7125</v>
       </c>
       <c r="P13">
-        <v>5114651.6071</v>
+        <v>222.52282</v>
       </c>
       <c r="Q13">
-        <v>26336324.388</v>
+        <v>1611.68342</v>
       </c>
       <c r="R13">
-        <v>1062.33061</v>
+        <v>86.453777</v>
       </c>
       <c r="S13">
-        <v>639.92233</v>
+        <v>72.96200199999998</v>
       </c>
       <c r="T13">
-        <v>625437850</v>
+        <v>32733.461</v>
       </c>
       <c r="U13">
-        <v>40718105.96</v>
+        <v>4353.765100000001</v>
       </c>
       <c r="V13">
-        <v>552.09223</v>
+        <v>99.49325100000001</v>
       </c>
       <c r="W13">
-        <v>333.92859</v>
+        <v>146.60353</v>
       </c>
       <c r="X13">
-        <v>1836.715</v>
+        <v>148.615835</v>
       </c>
       <c r="Y13">
-        <v>540.2689699999999</v>
+        <v>334.34546</v>
       </c>
       <c r="Z13">
-        <v>584.18386</v>
+        <v>353.74891</v>
       </c>
       <c r="AA13">
-        <v>1976.8844</v>
+        <v>459.0884600000001</v>
       </c>
       <c r="AB13">
-        <v>2158.7314</v>
+        <v>423.18556</v>
       </c>
       <c r="AC13">
-        <v>688.07339</v>
+        <v>396.35921</v>
       </c>
       <c r="AD13">
-        <v>1253.73054</v>
+        <v>488.20244</v>
       </c>
       <c r="AE13">
-        <v>910.44229</v>
+        <v>283.78711</v>
       </c>
       <c r="AF13">
-        <v>136807693</v>
+        <v>402252.685</v>
       </c>
       <c r="AG13">
         <v>10</v>
@@ -1791,94 +1791,94 @@
         <v>90</v>
       </c>
       <c r="C14">
-        <v>16571193700</v>
+        <v>124022737</v>
       </c>
       <c r="D14">
-        <v>79573461330000</v>
+        <v>3723016.5</v>
       </c>
       <c r="E14">
-        <v>80511.00499999999</v>
+        <v>435.07973</v>
       </c>
       <c r="F14">
-        <v>2494.89189</v>
+        <v>14.1192627</v>
       </c>
       <c r="G14">
-        <v>149.06841</v>
+        <v>31.659881</v>
       </c>
       <c r="H14">
-        <v>99.980987</v>
+        <v>6.8642368</v>
       </c>
       <c r="I14">
-        <v>399.2386</v>
+        <v>54.105006</v>
       </c>
       <c r="J14">
-        <v>144.51851</v>
+        <v>33.007335</v>
       </c>
       <c r="K14">
-        <v>3707.9775</v>
+        <v>34.514484</v>
       </c>
       <c r="L14">
-        <v>2492.267</v>
+        <v>791.24776</v>
       </c>
       <c r="M14">
-        <v>14679.5688</v>
+        <v>75.77861</v>
       </c>
       <c r="N14">
-        <v>2405794170</v>
+        <v>1507326.05</v>
       </c>
       <c r="O14">
-        <v>217149200</v>
+        <v>9267.8694</v>
       </c>
       <c r="P14">
-        <v>5114651.6071</v>
+        <v>196.715372</v>
       </c>
       <c r="Q14">
-        <v>26336324.388</v>
+        <v>752.683487</v>
       </c>
       <c r="R14">
-        <v>1062.33061</v>
+        <v>76.954903</v>
       </c>
       <c r="S14">
-        <v>639.92233</v>
+        <v>57.510632</v>
       </c>
       <c r="T14">
-        <v>625437850</v>
+        <v>31721.791</v>
       </c>
       <c r="U14">
-        <v>40718105.96</v>
+        <v>3527.665822</v>
       </c>
       <c r="V14">
-        <v>552.09223</v>
+        <v>99.08427999999999</v>
       </c>
       <c r="W14">
-        <v>333.92859</v>
+        <v>142.77588</v>
       </c>
       <c r="X14">
-        <v>1836.715</v>
+        <v>125.806303</v>
       </c>
       <c r="Y14">
-        <v>540.2689699999999</v>
+        <v>328.50247</v>
       </c>
       <c r="Z14">
-        <v>584.18386</v>
+        <v>348.5815999999999</v>
       </c>
       <c r="AA14">
-        <v>1976.8844</v>
+        <v>438.9484699999999</v>
       </c>
       <c r="AB14">
-        <v>2158.7314</v>
+        <v>356.59391</v>
       </c>
       <c r="AC14">
-        <v>688.07339</v>
+        <v>394.5102499999999</v>
       </c>
       <c r="AD14">
-        <v>1253.73054</v>
+        <v>478.1798299999999</v>
       </c>
       <c r="AE14">
-        <v>910.44229</v>
+        <v>274.09814</v>
       </c>
       <c r="AF14">
-        <v>136807693</v>
+        <v>281548.984</v>
       </c>
       <c r="AG14">
         <v>10</v>
@@ -1892,94 +1892,94 @@
         <v>100</v>
       </c>
       <c r="C15">
-        <v>16571193700</v>
+        <v>49696.52</v>
       </c>
       <c r="D15">
-        <v>79573461330000</v>
+        <v>7441.2</v>
       </c>
       <c r="E15">
-        <v>80511.00499999999</v>
+        <v>0.25247321</v>
       </c>
       <c r="F15">
-        <v>2494.89189</v>
+        <v>5.9565311</v>
       </c>
       <c r="G15">
-        <v>149.06841</v>
+        <v>9.2090023</v>
       </c>
       <c r="H15">
-        <v>99.980987</v>
+        <v>0.20352204</v>
       </c>
       <c r="I15">
-        <v>399.2386</v>
+        <v>20.0445692</v>
       </c>
       <c r="J15">
-        <v>144.51851</v>
+        <v>9.178035900000001</v>
       </c>
       <c r="K15">
-        <v>3707.9775</v>
+        <v>0.042884756</v>
       </c>
       <c r="L15">
-        <v>2492.267</v>
+        <v>489.19402</v>
       </c>
       <c r="M15">
-        <v>14679.5688</v>
+        <v>17.5445364</v>
       </c>
       <c r="N15">
-        <v>2405794170</v>
+        <v>431897.986</v>
       </c>
       <c r="O15">
-        <v>217149200</v>
+        <v>7829.7165</v>
       </c>
       <c r="P15">
-        <v>5114651.6071</v>
+        <v>127.444186</v>
       </c>
       <c r="Q15">
-        <v>26336324.388</v>
+        <v>493.433195</v>
       </c>
       <c r="R15">
-        <v>1062.33061</v>
+        <v>54.41707900000002</v>
       </c>
       <c r="S15">
-        <v>639.92233</v>
+        <v>40.80323499999999</v>
       </c>
       <c r="T15">
-        <v>625437850</v>
+        <v>26772.833</v>
       </c>
       <c r="U15">
-        <v>40718105.96</v>
+        <v>2659.94661</v>
       </c>
       <c r="V15">
-        <v>552.09223</v>
+        <v>74.94904199999999</v>
       </c>
       <c r="W15">
-        <v>333.92859</v>
+        <v>133.15995</v>
       </c>
       <c r="X15">
-        <v>1836.715</v>
+        <v>97.018854</v>
       </c>
       <c r="Y15">
-        <v>540.2689699999999</v>
+        <v>311.7599</v>
       </c>
       <c r="Z15">
-        <v>584.18386</v>
+        <v>331.60458</v>
       </c>
       <c r="AA15">
-        <v>1976.8844</v>
+        <v>421.98093</v>
       </c>
       <c r="AB15">
-        <v>2158.7314</v>
+        <v>300.47459</v>
       </c>
       <c r="AC15">
-        <v>688.07339</v>
+        <v>389.78664</v>
       </c>
       <c r="AD15">
-        <v>1253.73054</v>
+        <v>469.3348</v>
       </c>
       <c r="AE15">
-        <v>910.44229</v>
+        <v>246.75997</v>
       </c>
       <c r="AF15">
-        <v>136807693</v>
+        <v>230716.1606</v>
       </c>
       <c r="AG15">
         <v>10</v>

</xml_diff>